<commit_message>
Changes in axial 2020-2s
</commit_message>
<xml_diff>
--- a/Contenido.xlsx
+++ b/Contenido.xlsx
@@ -177,12 +177,6 @@
     <t>6.5. Arcos tri-articulados</t>
   </si>
   <si>
-    <t>7.1. Conceptos de trabajo real, trabajo virtual, trabajo interno de deformación</t>
-  </si>
-  <si>
-    <t>7.2. Teoremas de Castigliano, Maxwell, Betti</t>
-  </si>
-  <si>
     <t>8.1. Cargas móviles</t>
   </si>
   <si>
@@ -217,6 +211,12 @@
   </si>
   <si>
     <t>9.5. Solución del sistema algebraico</t>
+  </si>
+  <si>
+    <t>7.1. Conceptos de trabajo externo, trabajo virtual, energía interna de deformación</t>
+  </si>
+  <si>
+    <t>7.2. Teorema de Castigliano</t>
   </si>
 </sst>
 </file>
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1039,24 +1039,24 @@
     </row>
     <row r="29" spans="3:5" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C29" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="3:5" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C30" s="25"/>
       <c r="D30" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="3:5" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C31" s="25"/>
       <c r="D31" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E31" s="5"/>
     </row>
@@ -1102,33 +1102,35 @@
         <v>44</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>52</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="3:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C38" s="21"/>
       <c r="D38" s="8" t="s">
-        <v>53</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="3:5" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C39" s="20" t="s">
         <v>45</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="3:5" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C40" s="20"/>
       <c r="D40" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="3:5" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C41" s="20"/>
       <c r="D41" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="3:5" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1136,35 +1138,35 @@
         <v>46</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="3:5" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C43" s="22"/>
       <c r="D43" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="3:5" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C44" s="22"/>
       <c r="D44" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="3:5" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C45" s="22"/>
       <c r="D45" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E45" s="5"/>
     </row>
     <row r="46" spans="3:5" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C46" s="22"/>
       <c r="D46" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E46" s="5"/>
     </row>

</xml_diff>